<commit_message>
2012-10-29 Pushing current log and new HTML format for Excel workbooks.
</commit_message>
<xml_diff>
--- a/NormalValues/CO2Transport.xlsx
+++ b/NormalValues/CO2Transport.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>CO2 Transport</t>
   </si>
@@ -92,7 +92,10 @@
     <t>p50</t>
   </si>
   <si>
-    <t>Work Area</t>
+    <t>Tissue (General)</t>
+  </si>
+  <si>
+    <t>Skeletal Muscle</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -561,14 +564,38 @@
         <v>45</v>
       </c>
       <c r="C10">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D10">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E10">
         <f>(C10*(F10+B10))/(B10*D10)</f>
-        <v>0.27777777777777779</v>
+        <v>0.76049382716049385</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
+      </c>
+      <c r="D11">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E11">
+        <f>(C11*(F11+B11))/(B11*D11)</f>
+        <v>0.4753086419753087</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>